<commit_message>
fixed id slicing 781bed92d18e07f813a710c1baf2c56070b78ed2
</commit_message>
<xml_diff>
--- a/ig/sd-suppr-extension-eclaire-condition-details-and-new-slice/StructureDefinition-eclaire-researchstudy.xlsx
+++ b/ig/sd-suppr-extension-eclaire-condition-details-and-new-slice/StructureDefinition-eclaire-researchstudy.xlsx
@@ -10,13 +10,13 @@
     <sheet name="Elements" r:id="rId4" sheetId="2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">Elements!$A$1:$AO$77</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">Elements!$A$1:$AO$85</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2886" uniqueCount="475">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3184" uniqueCount="504">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-10-06T06:48:32+00:00</t>
+    <t>2023-10-06T19:29:53+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -970,6 +970,79 @@
     <t>code MedDRA / MedDRA condition</t>
   </si>
   <si>
+    <t>ResearchStudy.condition:medDRACondition.id</t>
+  </si>
+  <si>
+    <t>ResearchStudy.condition.id</t>
+  </si>
+  <si>
+    <t>meddra-condition</t>
+  </si>
+  <si>
+    <t>ResearchStudy.condition:medDRACondition.extension</t>
+  </si>
+  <si>
+    <t>ResearchStudy.condition.extension</t>
+  </si>
+  <si>
+    <t>ResearchStudy.condition:medDRACondition.coding</t>
+  </si>
+  <si>
+    <t>ResearchStudy.condition.coding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coding
+</t>
+  </si>
+  <si>
+    <t>Code defined by a terminology system</t>
+  </si>
+  <si>
+    <t>A reference to a code defined by a terminology system.</t>
+  </si>
+  <si>
+    <t>Codes may be defined very casually in enumerations, or code lists, up to very formal definitions such as SNOMED CT - see the HL7 v3 Core Principles for more information.  Ordering of codings is undefined and SHALL NOT be used to infer meaning. Generally, at most only one of the coding values will be labeled as UserSelected = true.</t>
+  </si>
+  <si>
+    <t>Allows for alternative encodings within a code system, and translations to other code systems.</t>
+  </si>
+  <si>
+    <t>CodeableConcept.coding</t>
+  </si>
+  <si>
+    <t>C*E.1-8, C*E.10-22</t>
+  </si>
+  <si>
+    <t>union(., ./translation)</t>
+  </si>
+  <si>
+    <t>ResearchStudy.condition:medDRACondition.text</t>
+  </si>
+  <si>
+    <t>ResearchStudy.condition.text</t>
+  </si>
+  <si>
+    <t>Plain text representation of the concept</t>
+  </si>
+  <si>
+    <t>A human language representation of the concept as seen/selected/uttered by the user who entered the data and/or which represents the intended meaning of the user.</t>
+  </si>
+  <si>
+    <t>Very often the text is the same as a displayName of one of the codings.</t>
+  </si>
+  <si>
+    <t>The codes from the terminologies do not always capture the correct meaning with all the nuances of the human using them, or sometimes there is no appropriate code at all. In these cases, the text is used to capture the full meaning of the source.</t>
+  </si>
+  <si>
+    <t>CodeableConcept.text</t>
+  </si>
+  <si>
+    <t>C*E.9. But note many systems use C*E.2 for this</t>
+  </si>
+  <si>
+    <t>./originalText[mediaType/code="text/plain"]/data</t>
+  </si>
+  <si>
     <t>ResearchStudy.condition:diseaseCondition</t>
   </si>
   <si>
@@ -977,6 +1050,21 @@
   </si>
   <si>
     <t>condition de la pathologie / Disease Condition</t>
+  </si>
+  <si>
+    <t>ResearchStudy.condition:diseaseCondition.id</t>
+  </si>
+  <si>
+    <t>disease-condition</t>
+  </si>
+  <si>
+    <t>ResearchStudy.condition:diseaseCondition.extension</t>
+  </si>
+  <si>
+    <t>ResearchStudy.condition:diseaseCondition.coding</t>
+  </si>
+  <si>
+    <t>ResearchStudy.condition:diseaseCondition.text</t>
   </si>
   <si>
     <t>ResearchStudy.contact</t>
@@ -1805,7 +1893,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AO77"/>
+  <dimension ref="A1:AO85"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -6905,42 +6993,38 @@
         <v>305</v>
       </c>
       <c r="B44" t="s" s="2">
-        <v>293</v>
-      </c>
-      <c r="C44" t="s" s="2">
         <v>306</v>
       </c>
+      <c r="C44" s="2"/>
       <c r="D44" t="s" s="2">
         <v>37</v>
       </c>
       <c r="E44" s="2"/>
       <c r="F44" t="s" s="2">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="G44" t="s" s="2">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="H44" t="s" s="2">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="I44" t="s" s="2">
         <v>37</v>
       </c>
       <c r="J44" t="s" s="2">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>173</v>
+        <v>151</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>307</v>
+        <v>152</v>
       </c>
       <c r="M44" t="s" s="2">
-        <v>295</v>
-      </c>
-      <c r="N44" t="s" s="2">
-        <v>267</v>
-      </c>
+        <v>153</v>
+      </c>
+      <c r="N44" s="2"/>
       <c r="O44" s="2"/>
       <c r="P44" t="s" s="2">
         <v>37</v>
@@ -6950,7 +7034,7 @@
         <v>37</v>
       </c>
       <c r="S44" t="s" s="2">
-        <v>37</v>
+        <v>307</v>
       </c>
       <c r="T44" t="s" s="2">
         <v>37</v>
@@ -6965,13 +7049,13 @@
         <v>37</v>
       </c>
       <c r="X44" t="s" s="2">
-        <v>282</v>
+        <v>37</v>
       </c>
       <c r="Y44" t="s" s="2">
-        <v>296</v>
+        <v>37</v>
       </c>
       <c r="Z44" t="s" s="2">
-        <v>297</v>
+        <v>37</v>
       </c>
       <c r="AA44" t="s" s="2">
         <v>37</v>
@@ -6989,34 +7073,34 @@
         <v>37</v>
       </c>
       <c r="AF44" t="s" s="2">
-        <v>293</v>
+        <v>154</v>
       </c>
       <c r="AG44" t="s" s="2">
         <v>35</v>
       </c>
       <c r="AH44" t="s" s="2">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="AI44" t="s" s="2">
-        <v>59</v>
+        <v>37</v>
       </c>
       <c r="AJ44" t="s" s="2">
-        <v>60</v>
+        <v>37</v>
       </c>
       <c r="AK44" t="s" s="2">
-        <v>300</v>
+        <v>37</v>
       </c>
       <c r="AL44" t="s" s="2">
-        <v>271</v>
+        <v>37</v>
       </c>
       <c r="AM44" t="s" s="2">
-        <v>272</v>
+        <v>68</v>
       </c>
       <c r="AN44" t="s" s="2">
-        <v>301</v>
+        <v>37</v>
       </c>
       <c r="AO44" t="s" s="2">
-        <v>292</v>
+        <v>37</v>
       </c>
     </row>
     <row r="45" hidden="true">
@@ -7024,11 +7108,11 @@
         <v>308</v>
       </c>
       <c r="B45" t="s" s="2">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" t="s" s="2">
-        <v>37</v>
+        <v>94</v>
       </c>
       <c r="E45" s="2"/>
       <c r="F45" t="s" s="2">
@@ -7038,24 +7122,26 @@
         <v>36</v>
       </c>
       <c r="H45" t="s" s="2">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="I45" t="s" s="2">
         <v>37</v>
       </c>
       <c r="J45" t="s" s="2">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="K45" t="s" s="2">
-        <v>309</v>
+        <v>95</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>310</v>
+        <v>96</v>
       </c>
       <c r="M45" t="s" s="2">
-        <v>311</v>
-      </c>
-      <c r="N45" s="2"/>
+        <v>157</v>
+      </c>
+      <c r="N45" t="s" s="2">
+        <v>98</v>
+      </c>
       <c r="O45" s="2"/>
       <c r="P45" t="s" s="2">
         <v>37</v>
@@ -7092,19 +7178,19 @@
         <v>37</v>
       </c>
       <c r="AB45" t="s" s="2">
-        <v>37</v>
+        <v>99</v>
       </c>
       <c r="AC45" t="s" s="2">
-        <v>37</v>
+        <v>100</v>
       </c>
       <c r="AD45" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AE45" t="s" s="2">
-        <v>37</v>
+        <v>101</v>
       </c>
       <c r="AF45" t="s" s="2">
-        <v>308</v>
+        <v>158</v>
       </c>
       <c r="AG45" t="s" s="2">
         <v>35</v>
@@ -7116,19 +7202,19 @@
         <v>59</v>
       </c>
       <c r="AJ45" t="s" s="2">
-        <v>60</v>
+        <v>103</v>
       </c>
       <c r="AK45" t="s" s="2">
-        <v>312</v>
+        <v>37</v>
       </c>
       <c r="AL45" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AM45" t="s" s="2">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="AN45" t="s" s="2">
-        <v>313</v>
+        <v>37</v>
       </c>
       <c r="AO45" t="s" s="2">
         <v>37</v>
@@ -7136,10 +7222,10 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="B46" t="s" s="2">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" t="s" s="2">
@@ -7150,7 +7236,7 @@
         <v>35</v>
       </c>
       <c r="G46" t="s" s="2">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="H46" t="s" s="2">
         <v>37</v>
@@ -7159,19 +7245,23 @@
         <v>37</v>
       </c>
       <c r="J46" t="s" s="2">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>151</v>
+        <v>312</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>152</v>
+        <v>313</v>
       </c>
       <c r="M46" t="s" s="2">
-        <v>153</v>
-      </c>
-      <c r="N46" s="2"/>
-      <c r="O46" s="2"/>
+        <v>314</v>
+      </c>
+      <c r="N46" t="s" s="2">
+        <v>315</v>
+      </c>
+      <c r="O46" t="s" s="2">
+        <v>316</v>
+      </c>
       <c r="P46" t="s" s="2">
         <v>37</v>
       </c>
@@ -7219,28 +7309,28 @@
         <v>37</v>
       </c>
       <c r="AF46" t="s" s="2">
-        <v>154</v>
+        <v>317</v>
       </c>
       <c r="AG46" t="s" s="2">
         <v>35</v>
       </c>
       <c r="AH46" t="s" s="2">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="AI46" t="s" s="2">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="AJ46" t="s" s="2">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="AK46" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AL46" t="s" s="2">
-        <v>37</v>
+        <v>318</v>
       </c>
       <c r="AM46" t="s" s="2">
-        <v>68</v>
+        <v>319</v>
       </c>
       <c r="AN46" t="s" s="2">
         <v>37</v>
@@ -7251,21 +7341,21 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>315</v>
+        <v>320</v>
       </c>
       <c r="B47" t="s" s="2">
-        <v>315</v>
+        <v>321</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" t="s" s="2">
-        <v>94</v>
+        <v>37</v>
       </c>
       <c r="E47" s="2"/>
       <c r="F47" t="s" s="2">
         <v>35</v>
       </c>
       <c r="G47" t="s" s="2">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="H47" t="s" s="2">
         <v>37</v>
@@ -7274,21 +7364,23 @@
         <v>37</v>
       </c>
       <c r="J47" t="s" s="2">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>95</v>
+        <v>151</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>96</v>
+        <v>322</v>
       </c>
       <c r="M47" t="s" s="2">
-        <v>157</v>
+        <v>323</v>
       </c>
       <c r="N47" t="s" s="2">
-        <v>98</v>
-      </c>
-      <c r="O47" s="2"/>
+        <v>324</v>
+      </c>
+      <c r="O47" t="s" s="2">
+        <v>325</v>
+      </c>
       <c r="P47" t="s" s="2">
         <v>37</v>
       </c>
@@ -7324,40 +7416,40 @@
         <v>37</v>
       </c>
       <c r="AB47" t="s" s="2">
-        <v>99</v>
+        <v>37</v>
       </c>
       <c r="AC47" t="s" s="2">
-        <v>100</v>
+        <v>37</v>
       </c>
       <c r="AD47" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AE47" t="s" s="2">
-        <v>101</v>
+        <v>37</v>
       </c>
       <c r="AF47" t="s" s="2">
-        <v>158</v>
+        <v>326</v>
       </c>
       <c r="AG47" t="s" s="2">
         <v>35</v>
       </c>
       <c r="AH47" t="s" s="2">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="AI47" t="s" s="2">
         <v>59</v>
       </c>
       <c r="AJ47" t="s" s="2">
-        <v>103</v>
+        <v>60</v>
       </c>
       <c r="AK47" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AL47" t="s" s="2">
-        <v>37</v>
+        <v>327</v>
       </c>
       <c r="AM47" t="s" s="2">
-        <v>61</v>
+        <v>328</v>
       </c>
       <c r="AN47" t="s" s="2">
         <v>37</v>
@@ -7368,13 +7460,13 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>316</v>
+        <v>329</v>
       </c>
       <c r="B48" t="s" s="2">
-        <v>315</v>
+        <v>293</v>
       </c>
       <c r="C48" t="s" s="2">
-        <v>317</v>
+        <v>330</v>
       </c>
       <c r="D48" t="s" s="2">
         <v>37</v>
@@ -7384,7 +7476,7 @@
         <v>35</v>
       </c>
       <c r="G48" t="s" s="2">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="H48" t="s" s="2">
         <v>48</v>
@@ -7393,18 +7485,20 @@
         <v>37</v>
       </c>
       <c r="J48" t="s" s="2">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>318</v>
+        <v>173</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>319</v>
+        <v>331</v>
       </c>
       <c r="M48" t="s" s="2">
-        <v>320</v>
-      </c>
-      <c r="N48" s="2"/>
+        <v>295</v>
+      </c>
+      <c r="N48" t="s" s="2">
+        <v>267</v>
+      </c>
       <c r="O48" s="2"/>
       <c r="P48" t="s" s="2">
         <v>37</v>
@@ -7429,13 +7523,13 @@
         <v>37</v>
       </c>
       <c r="X48" t="s" s="2">
-        <v>37</v>
+        <v>282</v>
       </c>
       <c r="Y48" t="s" s="2">
-        <v>37</v>
+        <v>296</v>
       </c>
       <c r="Z48" t="s" s="2">
-        <v>37</v>
+        <v>297</v>
       </c>
       <c r="AA48" t="s" s="2">
         <v>37</v>
@@ -7453,7 +7547,7 @@
         <v>37</v>
       </c>
       <c r="AF48" t="s" s="2">
-        <v>158</v>
+        <v>293</v>
       </c>
       <c r="AG48" t="s" s="2">
         <v>35</v>
@@ -7465,46 +7559,44 @@
         <v>59</v>
       </c>
       <c r="AJ48" t="s" s="2">
-        <v>103</v>
+        <v>60</v>
       </c>
       <c r="AK48" t="s" s="2">
-        <v>37</v>
+        <v>300</v>
       </c>
       <c r="AL48" t="s" s="2">
-        <v>37</v>
+        <v>271</v>
       </c>
       <c r="AM48" t="s" s="2">
-        <v>37</v>
+        <v>272</v>
       </c>
       <c r="AN48" t="s" s="2">
-        <v>37</v>
+        <v>301</v>
       </c>
       <c r="AO48" t="s" s="2">
-        <v>37</v>
+        <v>292</v>
       </c>
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>321</v>
+        <v>332</v>
       </c>
       <c r="B49" t="s" s="2">
-        <v>315</v>
-      </c>
-      <c r="C49" t="s" s="2">
-        <v>322</v>
-      </c>
+        <v>306</v>
+      </c>
+      <c r="C49" s="2"/>
       <c r="D49" t="s" s="2">
         <v>37</v>
       </c>
       <c r="E49" s="2"/>
       <c r="F49" t="s" s="2">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="G49" t="s" s="2">
         <v>47</v>
       </c>
       <c r="H49" t="s" s="2">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="I49" t="s" s="2">
         <v>37</v>
@@ -7513,13 +7605,13 @@
         <v>37</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>323</v>
+        <v>151</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>324</v>
+        <v>152</v>
       </c>
       <c r="M49" t="s" s="2">
-        <v>325</v>
+        <v>153</v>
       </c>
       <c r="N49" s="2"/>
       <c r="O49" s="2"/>
@@ -7531,7 +7623,7 @@
         <v>37</v>
       </c>
       <c r="S49" t="s" s="2">
-        <v>37</v>
+        <v>333</v>
       </c>
       <c r="T49" t="s" s="2">
         <v>37</v>
@@ -7570,19 +7662,19 @@
         <v>37</v>
       </c>
       <c r="AF49" t="s" s="2">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="AG49" t="s" s="2">
         <v>35</v>
       </c>
       <c r="AH49" t="s" s="2">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="AI49" t="s" s="2">
-        <v>59</v>
+        <v>37</v>
       </c>
       <c r="AJ49" t="s" s="2">
-        <v>103</v>
+        <v>37</v>
       </c>
       <c r="AK49" t="s" s="2">
         <v>37</v>
@@ -7591,7 +7683,7 @@
         <v>37</v>
       </c>
       <c r="AM49" t="s" s="2">
-        <v>37</v>
+        <v>68</v>
       </c>
       <c r="AN49" t="s" s="2">
         <v>37</v>
@@ -7602,26 +7694,24 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>326</v>
+        <v>334</v>
       </c>
       <c r="B50" t="s" s="2">
-        <v>315</v>
-      </c>
-      <c r="C50" t="s" s="2">
-        <v>327</v>
-      </c>
+        <v>309</v>
+      </c>
+      <c r="C50" s="2"/>
       <c r="D50" t="s" s="2">
-        <v>37</v>
+        <v>94</v>
       </c>
       <c r="E50" s="2"/>
       <c r="F50" t="s" s="2">
         <v>35</v>
       </c>
       <c r="G50" t="s" s="2">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="H50" t="s" s="2">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="I50" t="s" s="2">
         <v>37</v>
@@ -7630,15 +7720,17 @@
         <v>37</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>328</v>
+        <v>95</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>329</v>
+        <v>96</v>
       </c>
       <c r="M50" t="s" s="2">
-        <v>330</v>
-      </c>
-      <c r="N50" s="2"/>
+        <v>157</v>
+      </c>
+      <c r="N50" t="s" s="2">
+        <v>98</v>
+      </c>
       <c r="O50" s="2"/>
       <c r="P50" t="s" s="2">
         <v>37</v>
@@ -7675,16 +7767,16 @@
         <v>37</v>
       </c>
       <c r="AB50" t="s" s="2">
-        <v>37</v>
+        <v>99</v>
       </c>
       <c r="AC50" t="s" s="2">
-        <v>37</v>
+        <v>100</v>
       </c>
       <c r="AD50" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AE50" t="s" s="2">
-        <v>37</v>
+        <v>101</v>
       </c>
       <c r="AF50" t="s" s="2">
         <v>158</v>
@@ -7708,7 +7800,7 @@
         <v>37</v>
       </c>
       <c r="AM50" t="s" s="2">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="AN50" t="s" s="2">
         <v>37</v>
@@ -7719,14 +7811,12 @@
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="B51" t="s" s="2">
-        <v>315</v>
-      </c>
-      <c r="C51" t="s" s="2">
-        <v>332</v>
-      </c>
+        <v>311</v>
+      </c>
+      <c r="C51" s="2"/>
       <c r="D51" t="s" s="2">
         <v>37</v>
       </c>
@@ -7735,7 +7825,7 @@
         <v>35</v>
       </c>
       <c r="G51" t="s" s="2">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="H51" t="s" s="2">
         <v>37</v>
@@ -7744,19 +7834,23 @@
         <v>37</v>
       </c>
       <c r="J51" t="s" s="2">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>333</v>
+        <v>312</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>334</v>
+        <v>313</v>
       </c>
       <c r="M51" t="s" s="2">
-        <v>335</v>
-      </c>
-      <c r="N51" s="2"/>
-      <c r="O51" s="2"/>
+        <v>314</v>
+      </c>
+      <c r="N51" t="s" s="2">
+        <v>315</v>
+      </c>
+      <c r="O51" t="s" s="2">
+        <v>316</v>
+      </c>
       <c r="P51" t="s" s="2">
         <v>37</v>
       </c>
@@ -7804,7 +7898,7 @@
         <v>37</v>
       </c>
       <c r="AF51" t="s" s="2">
-        <v>158</v>
+        <v>317</v>
       </c>
       <c r="AG51" t="s" s="2">
         <v>35</v>
@@ -7816,16 +7910,16 @@
         <v>59</v>
       </c>
       <c r="AJ51" t="s" s="2">
-        <v>103</v>
+        <v>60</v>
       </c>
       <c r="AK51" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AL51" t="s" s="2">
-        <v>37</v>
+        <v>318</v>
       </c>
       <c r="AM51" t="s" s="2">
-        <v>37</v>
+        <v>319</v>
       </c>
       <c r="AN51" t="s" s="2">
         <v>37</v>
@@ -7839,7 +7933,7 @@
         <v>336</v>
       </c>
       <c r="B52" t="s" s="2">
-        <v>336</v>
+        <v>321</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" t="s" s="2">
@@ -7865,15 +7959,17 @@
         <v>151</v>
       </c>
       <c r="L52" t="s" s="2">
-        <v>337</v>
+        <v>322</v>
       </c>
       <c r="M52" t="s" s="2">
-        <v>338</v>
+        <v>323</v>
       </c>
       <c r="N52" t="s" s="2">
-        <v>339</v>
-      </c>
-      <c r="O52" s="2"/>
+        <v>324</v>
+      </c>
+      <c r="O52" t="s" s="2">
+        <v>325</v>
+      </c>
       <c r="P52" t="s" s="2">
         <v>37</v>
       </c>
@@ -7921,7 +8017,7 @@
         <v>37</v>
       </c>
       <c r="AF52" t="s" s="2">
-        <v>340</v>
+        <v>326</v>
       </c>
       <c r="AG52" t="s" s="2">
         <v>35</v>
@@ -7939,10 +8035,10 @@
         <v>37</v>
       </c>
       <c r="AL52" t="s" s="2">
-        <v>37</v>
+        <v>327</v>
       </c>
       <c r="AM52" t="s" s="2">
-        <v>68</v>
+        <v>328</v>
       </c>
       <c r="AN52" t="s" s="2">
         <v>37</v>
@@ -7953,10 +8049,10 @@
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="B53" t="s" s="2">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" t="s" s="2">
@@ -7970,7 +8066,7 @@
         <v>36</v>
       </c>
       <c r="H53" t="s" s="2">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="I53" t="s" s="2">
         <v>37</v>
@@ -7979,13 +8075,13 @@
         <v>48</v>
       </c>
       <c r="K53" t="s" s="2">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="L53" t="s" s="2">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="M53" t="s" s="2">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="N53" s="2"/>
       <c r="O53" s="2"/>
@@ -8036,7 +8132,7 @@
         <v>37</v>
       </c>
       <c r="AF53" t="s" s="2">
-        <v>345</v>
+        <v>337</v>
       </c>
       <c r="AG53" t="s" s="2">
         <v>35</v>
@@ -8048,19 +8144,19 @@
         <v>59</v>
       </c>
       <c r="AJ53" t="s" s="2">
-        <v>346</v>
+        <v>60</v>
       </c>
       <c r="AK53" t="s" s="2">
-        <v>37</v>
+        <v>341</v>
       </c>
       <c r="AL53" t="s" s="2">
-        <v>347</v>
+        <v>37</v>
       </c>
       <c r="AM53" t="s" s="2">
-        <v>348</v>
+        <v>68</v>
       </c>
       <c r="AN53" t="s" s="2">
-        <v>37</v>
+        <v>342</v>
       </c>
       <c r="AO53" t="s" s="2">
         <v>37</v>
@@ -8068,10 +8164,10 @@
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="B54" t="s" s="2">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" t="s" s="2">
@@ -8082,7 +8178,7 @@
         <v>35</v>
       </c>
       <c r="G54" t="s" s="2">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="H54" t="s" s="2">
         <v>37</v>
@@ -8094,17 +8190,15 @@
         <v>37</v>
       </c>
       <c r="K54" t="s" s="2">
-        <v>350</v>
+        <v>151</v>
       </c>
       <c r="L54" t="s" s="2">
-        <v>351</v>
+        <v>152</v>
       </c>
       <c r="M54" t="s" s="2">
-        <v>352</v>
-      </c>
-      <c r="N54" t="s" s="2">
-        <v>353</v>
-      </c>
+        <v>153</v>
+      </c>
+      <c r="N54" s="2"/>
       <c r="O54" s="2"/>
       <c r="P54" t="s" s="2">
         <v>37</v>
@@ -8153,22 +8247,22 @@
         <v>37</v>
       </c>
       <c r="AF54" t="s" s="2">
-        <v>349</v>
+        <v>154</v>
       </c>
       <c r="AG54" t="s" s="2">
         <v>35</v>
       </c>
       <c r="AH54" t="s" s="2">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="AI54" t="s" s="2">
-        <v>59</v>
+        <v>37</v>
       </c>
       <c r="AJ54" t="s" s="2">
-        <v>60</v>
+        <v>37</v>
       </c>
       <c r="AK54" t="s" s="2">
-        <v>354</v>
+        <v>37</v>
       </c>
       <c r="AL54" t="s" s="2">
         <v>37</v>
@@ -8177,7 +8271,7 @@
         <v>68</v>
       </c>
       <c r="AN54" t="s" s="2">
-        <v>355</v>
+        <v>37</v>
       </c>
       <c r="AO54" t="s" s="2">
         <v>37</v>
@@ -8185,14 +8279,14 @@
     </row>
     <row r="55" hidden="true">
       <c r="A55" t="s" s="2">
-        <v>356</v>
+        <v>344</v>
       </c>
       <c r="B55" t="s" s="2">
-        <v>356</v>
+        <v>344</v>
       </c>
       <c r="C55" s="2"/>
       <c r="D55" t="s" s="2">
-        <v>37</v>
+        <v>94</v>
       </c>
       <c r="E55" s="2"/>
       <c r="F55" t="s" s="2">
@@ -8208,19 +8302,19 @@
         <v>37</v>
       </c>
       <c r="J55" t="s" s="2">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="K55" t="s" s="2">
-        <v>173</v>
+        <v>95</v>
       </c>
       <c r="L55" t="s" s="2">
-        <v>357</v>
+        <v>96</v>
       </c>
       <c r="M55" t="s" s="2">
-        <v>358</v>
+        <v>157</v>
       </c>
       <c r="N55" t="s" s="2">
-        <v>267</v>
+        <v>98</v>
       </c>
       <c r="O55" s="2"/>
       <c r="P55" t="s" s="2">
@@ -8246,10 +8340,10 @@
         <v>37</v>
       </c>
       <c r="X55" t="s" s="2">
-        <v>282</v>
+        <v>37</v>
       </c>
       <c r="Y55" t="s" s="2">
-        <v>359</v>
+        <v>37</v>
       </c>
       <c r="Z55" t="s" s="2">
         <v>37</v>
@@ -8258,19 +8352,19 @@
         <v>37</v>
       </c>
       <c r="AB55" t="s" s="2">
-        <v>37</v>
+        <v>99</v>
       </c>
       <c r="AC55" t="s" s="2">
-        <v>37</v>
+        <v>100</v>
       </c>
       <c r="AD55" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AE55" t="s" s="2">
-        <v>37</v>
+        <v>101</v>
       </c>
       <c r="AF55" t="s" s="2">
-        <v>356</v>
+        <v>158</v>
       </c>
       <c r="AG55" t="s" s="2">
         <v>35</v>
@@ -8282,19 +8376,19 @@
         <v>59</v>
       </c>
       <c r="AJ55" t="s" s="2">
-        <v>60</v>
+        <v>103</v>
       </c>
       <c r="AK55" t="s" s="2">
-        <v>360</v>
+        <v>37</v>
       </c>
       <c r="AL55" t="s" s="2">
-        <v>271</v>
+        <v>37</v>
       </c>
       <c r="AM55" t="s" s="2">
-        <v>272</v>
+        <v>61</v>
       </c>
       <c r="AN55" t="s" s="2">
-        <v>361</v>
+        <v>37</v>
       </c>
       <c r="AO55" t="s" s="2">
         <v>37</v>
@@ -8302,12 +8396,14 @@
     </row>
     <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>362</v>
+        <v>345</v>
       </c>
       <c r="B56" t="s" s="2">
-        <v>362</v>
-      </c>
-      <c r="C56" s="2"/>
+        <v>344</v>
+      </c>
+      <c r="C56" t="s" s="2">
+        <v>346</v>
+      </c>
       <c r="D56" t="s" s="2">
         <v>37</v>
       </c>
@@ -8316,7 +8412,7 @@
         <v>35</v>
       </c>
       <c r="G56" t="s" s="2">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="H56" t="s" s="2">
         <v>48</v>
@@ -8325,20 +8421,18 @@
         <v>37</v>
       </c>
       <c r="J56" t="s" s="2">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="K56" t="s" s="2">
-        <v>173</v>
+        <v>347</v>
       </c>
       <c r="L56" t="s" s="2">
-        <v>363</v>
+        <v>348</v>
       </c>
       <c r="M56" t="s" s="2">
-        <v>364</v>
-      </c>
-      <c r="N56" t="s" s="2">
-        <v>267</v>
-      </c>
+        <v>349</v>
+      </c>
+      <c r="N56" s="2"/>
       <c r="O56" s="2"/>
       <c r="P56" t="s" s="2">
         <v>37</v>
@@ -8363,13 +8457,13 @@
         <v>37</v>
       </c>
       <c r="X56" t="s" s="2">
-        <v>178</v>
+        <v>37</v>
       </c>
       <c r="Y56" t="s" s="2">
-        <v>365</v>
+        <v>37</v>
       </c>
       <c r="Z56" t="s" s="2">
-        <v>366</v>
+        <v>37</v>
       </c>
       <c r="AA56" t="s" s="2">
         <v>37</v>
@@ -8387,7 +8481,7 @@
         <v>37</v>
       </c>
       <c r="AF56" t="s" s="2">
-        <v>362</v>
+        <v>158</v>
       </c>
       <c r="AG56" t="s" s="2">
         <v>35</v>
@@ -8399,16 +8493,16 @@
         <v>59</v>
       </c>
       <c r="AJ56" t="s" s="2">
-        <v>60</v>
+        <v>103</v>
       </c>
       <c r="AK56" t="s" s="2">
-        <v>367</v>
+        <v>37</v>
       </c>
       <c r="AL56" t="s" s="2">
-        <v>271</v>
+        <v>37</v>
       </c>
       <c r="AM56" t="s" s="2">
-        <v>272</v>
+        <v>37</v>
       </c>
       <c r="AN56" t="s" s="2">
         <v>37</v>
@@ -8419,12 +8513,14 @@
     </row>
     <row r="57" hidden="true">
       <c r="A57" t="s" s="2">
-        <v>368</v>
+        <v>350</v>
       </c>
       <c r="B57" t="s" s="2">
-        <v>368</v>
-      </c>
-      <c r="C57" s="2"/>
+        <v>344</v>
+      </c>
+      <c r="C57" t="s" s="2">
+        <v>351</v>
+      </c>
       <c r="D57" t="s" s="2">
         <v>37</v>
       </c>
@@ -8445,17 +8541,15 @@
         <v>37</v>
       </c>
       <c r="K57" t="s" s="2">
-        <v>369</v>
+        <v>352</v>
       </c>
       <c r="L57" t="s" s="2">
-        <v>370</v>
+        <v>353</v>
       </c>
       <c r="M57" t="s" s="2">
-        <v>371</v>
-      </c>
-      <c r="N57" t="s" s="2">
-        <v>372</v>
-      </c>
+        <v>354</v>
+      </c>
+      <c r="N57" s="2"/>
       <c r="O57" s="2"/>
       <c r="P57" t="s" s="2">
         <v>37</v>
@@ -8504,31 +8598,31 @@
         <v>37</v>
       </c>
       <c r="AF57" t="s" s="2">
-        <v>368</v>
+        <v>158</v>
       </c>
       <c r="AG57" t="s" s="2">
         <v>35</v>
       </c>
       <c r="AH57" t="s" s="2">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="AI57" t="s" s="2">
         <v>59</v>
       </c>
       <c r="AJ57" t="s" s="2">
-        <v>60</v>
+        <v>103</v>
       </c>
       <c r="AK57" t="s" s="2">
-        <v>373</v>
+        <v>37</v>
       </c>
       <c r="AL57" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AM57" t="s" s="2">
-        <v>68</v>
+        <v>37</v>
       </c>
       <c r="AN57" t="s" s="2">
-        <v>374</v>
+        <v>37</v>
       </c>
       <c r="AO57" t="s" s="2">
         <v>37</v>
@@ -8536,21 +8630,23 @@
     </row>
     <row r="58" hidden="true">
       <c r="A58" t="s" s="2">
-        <v>375</v>
+        <v>355</v>
       </c>
       <c r="B58" t="s" s="2">
-        <v>375</v>
-      </c>
-      <c r="C58" s="2"/>
+        <v>344</v>
+      </c>
+      <c r="C58" t="s" s="2">
+        <v>356</v>
+      </c>
       <c r="D58" t="s" s="2">
-        <v>376</v>
+        <v>37</v>
       </c>
       <c r="E58" s="2"/>
       <c r="F58" t="s" s="2">
         <v>35</v>
       </c>
       <c r="G58" t="s" s="2">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="H58" t="s" s="2">
         <v>48</v>
@@ -8559,20 +8655,18 @@
         <v>37</v>
       </c>
       <c r="J58" t="s" s="2">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="K58" t="s" s="2">
-        <v>377</v>
+        <v>357</v>
       </c>
       <c r="L58" t="s" s="2">
-        <v>378</v>
+        <v>358</v>
       </c>
       <c r="M58" t="s" s="2">
-        <v>379</v>
-      </c>
-      <c r="N58" t="s" s="2">
-        <v>380</v>
-      </c>
+        <v>359</v>
+      </c>
+      <c r="N58" s="2"/>
       <c r="O58" s="2"/>
       <c r="P58" t="s" s="2">
         <v>37</v>
@@ -8621,7 +8715,7 @@
         <v>37</v>
       </c>
       <c r="AF58" t="s" s="2">
-        <v>375</v>
+        <v>158</v>
       </c>
       <c r="AG58" t="s" s="2">
         <v>35</v>
@@ -8633,34 +8727,36 @@
         <v>59</v>
       </c>
       <c r="AJ58" t="s" s="2">
-        <v>219</v>
+        <v>103</v>
       </c>
       <c r="AK58" t="s" s="2">
-        <v>381</v>
+        <v>37</v>
       </c>
       <c r="AL58" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AM58" t="s" s="2">
-        <v>382</v>
+        <v>37</v>
       </c>
       <c r="AN58" t="s" s="2">
-        <v>383</v>
+        <v>37</v>
       </c>
       <c r="AO58" t="s" s="2">
-        <v>384</v>
+        <v>37</v>
       </c>
     </row>
     <row r="59" hidden="true">
       <c r="A59" t="s" s="2">
-        <v>385</v>
+        <v>360</v>
       </c>
       <c r="B59" t="s" s="2">
-        <v>385</v>
-      </c>
-      <c r="C59" s="2"/>
+        <v>344</v>
+      </c>
+      <c r="C59" t="s" s="2">
+        <v>361</v>
+      </c>
       <c r="D59" t="s" s="2">
-        <v>386</v>
+        <v>37</v>
       </c>
       <c r="E59" s="2"/>
       <c r="F59" t="s" s="2">
@@ -8676,20 +8772,18 @@
         <v>37</v>
       </c>
       <c r="J59" t="s" s="2">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="K59" t="s" s="2">
-        <v>204</v>
+        <v>362</v>
       </c>
       <c r="L59" t="s" s="2">
-        <v>387</v>
+        <v>363</v>
       </c>
       <c r="M59" t="s" s="2">
-        <v>388</v>
-      </c>
-      <c r="N59" t="s" s="2">
-        <v>207</v>
-      </c>
+        <v>364</v>
+      </c>
+      <c r="N59" s="2"/>
       <c r="O59" s="2"/>
       <c r="P59" t="s" s="2">
         <v>37</v>
@@ -8738,42 +8832,42 @@
         <v>37</v>
       </c>
       <c r="AF59" t="s" s="2">
-        <v>385</v>
+        <v>158</v>
       </c>
       <c r="AG59" t="s" s="2">
         <v>35</v>
       </c>
       <c r="AH59" t="s" s="2">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="AI59" t="s" s="2">
         <v>59</v>
       </c>
       <c r="AJ59" t="s" s="2">
-        <v>209</v>
+        <v>103</v>
       </c>
       <c r="AK59" t="s" s="2">
-        <v>389</v>
+        <v>37</v>
       </c>
       <c r="AL59" t="s" s="2">
-        <v>390</v>
+        <v>37</v>
       </c>
       <c r="AM59" t="s" s="2">
-        <v>391</v>
+        <v>37</v>
       </c>
       <c r="AN59" t="s" s="2">
-        <v>392</v>
+        <v>37</v>
       </c>
       <c r="AO59" t="s" s="2">
-        <v>393</v>
+        <v>37</v>
       </c>
     </row>
     <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
-        <v>394</v>
+        <v>365</v>
       </c>
       <c r="B60" t="s" s="2">
-        <v>394</v>
+        <v>365</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" t="s" s="2">
@@ -8787,7 +8881,7 @@
         <v>47</v>
       </c>
       <c r="H60" t="s" s="2">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="I60" t="s" s="2">
         <v>37</v>
@@ -8796,16 +8890,16 @@
         <v>48</v>
       </c>
       <c r="K60" t="s" s="2">
-        <v>214</v>
+        <v>151</v>
       </c>
       <c r="L60" t="s" s="2">
-        <v>395</v>
+        <v>366</v>
       </c>
       <c r="M60" t="s" s="2">
-        <v>396</v>
+        <v>367</v>
       </c>
       <c r="N60" t="s" s="2">
-        <v>244</v>
+        <v>368</v>
       </c>
       <c r="O60" s="2"/>
       <c r="P60" t="s" s="2">
@@ -8855,7 +8949,7 @@
         <v>37</v>
       </c>
       <c r="AF60" t="s" s="2">
-        <v>394</v>
+        <v>369</v>
       </c>
       <c r="AG60" t="s" s="2">
         <v>35</v>
@@ -8867,30 +8961,30 @@
         <v>59</v>
       </c>
       <c r="AJ60" t="s" s="2">
-        <v>219</v>
+        <v>60</v>
       </c>
       <c r="AK60" t="s" s="2">
-        <v>397</v>
+        <v>37</v>
       </c>
       <c r="AL60" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AM60" t="s" s="2">
-        <v>398</v>
+        <v>68</v>
       </c>
       <c r="AN60" t="s" s="2">
-        <v>399</v>
+        <v>37</v>
       </c>
       <c r="AO60" t="s" s="2">
-        <v>400</v>
+        <v>37</v>
       </c>
     </row>
     <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
-        <v>401</v>
+        <v>370</v>
       </c>
       <c r="B61" t="s" s="2">
-        <v>401</v>
+        <v>370</v>
       </c>
       <c r="C61" s="2"/>
       <c r="D61" t="s" s="2">
@@ -8901,7 +8995,7 @@
         <v>35</v>
       </c>
       <c r="G61" t="s" s="2">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="H61" t="s" s="2">
         <v>37</v>
@@ -8913,17 +9007,15 @@
         <v>48</v>
       </c>
       <c r="K61" t="s" s="2">
-        <v>402</v>
+        <v>371</v>
       </c>
       <c r="L61" t="s" s="2">
-        <v>403</v>
+        <v>372</v>
       </c>
       <c r="M61" t="s" s="2">
-        <v>404</v>
-      </c>
-      <c r="N61" t="s" s="2">
-        <v>244</v>
-      </c>
+        <v>373</v>
+      </c>
+      <c r="N61" s="2"/>
       <c r="O61" s="2"/>
       <c r="P61" t="s" s="2">
         <v>37</v>
@@ -8972,42 +9064,42 @@
         <v>37</v>
       </c>
       <c r="AF61" t="s" s="2">
-        <v>401</v>
+        <v>374</v>
       </c>
       <c r="AG61" t="s" s="2">
         <v>35</v>
       </c>
       <c r="AH61" t="s" s="2">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="AI61" t="s" s="2">
         <v>59</v>
       </c>
       <c r="AJ61" t="s" s="2">
-        <v>219</v>
+        <v>375</v>
       </c>
       <c r="AK61" t="s" s="2">
-        <v>405</v>
+        <v>37</v>
       </c>
       <c r="AL61" t="s" s="2">
-        <v>37</v>
+        <v>376</v>
       </c>
       <c r="AM61" t="s" s="2">
-        <v>406</v>
+        <v>377</v>
       </c>
       <c r="AN61" t="s" s="2">
-        <v>407</v>
+        <v>37</v>
       </c>
       <c r="AO61" t="s" s="2">
-        <v>400</v>
+        <v>37</v>
       </c>
     </row>
     <row r="62" hidden="true">
       <c r="A62" t="s" s="2">
-        <v>408</v>
+        <v>378</v>
       </c>
       <c r="B62" t="s" s="2">
-        <v>408</v>
+        <v>378</v>
       </c>
       <c r="C62" s="2"/>
       <c r="D62" t="s" s="2">
@@ -9021,25 +9113,25 @@
         <v>36</v>
       </c>
       <c r="H62" t="s" s="2">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="I62" t="s" s="2">
         <v>37</v>
       </c>
       <c r="J62" t="s" s="2">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="K62" t="s" s="2">
-        <v>409</v>
+        <v>379</v>
       </c>
       <c r="L62" t="s" s="2">
-        <v>410</v>
+        <v>380</v>
       </c>
       <c r="M62" t="s" s="2">
-        <v>411</v>
+        <v>381</v>
       </c>
       <c r="N62" t="s" s="2">
-        <v>244</v>
+        <v>382</v>
       </c>
       <c r="O62" s="2"/>
       <c r="P62" t="s" s="2">
@@ -9089,7 +9181,7 @@
         <v>37</v>
       </c>
       <c r="AF62" t="s" s="2">
-        <v>408</v>
+        <v>378</v>
       </c>
       <c r="AG62" t="s" s="2">
         <v>35</v>
@@ -9101,30 +9193,30 @@
         <v>59</v>
       </c>
       <c r="AJ62" t="s" s="2">
-        <v>219</v>
+        <v>60</v>
       </c>
       <c r="AK62" t="s" s="2">
-        <v>412</v>
+        <v>383</v>
       </c>
       <c r="AL62" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AM62" t="s" s="2">
-        <v>406</v>
+        <v>68</v>
       </c>
       <c r="AN62" t="s" s="2">
-        <v>413</v>
+        <v>384</v>
       </c>
       <c r="AO62" t="s" s="2">
-        <v>414</v>
+        <v>37</v>
       </c>
     </row>
     <row r="63" hidden="true">
       <c r="A63" t="s" s="2">
-        <v>415</v>
+        <v>385</v>
       </c>
       <c r="B63" t="s" s="2">
-        <v>415</v>
+        <v>385</v>
       </c>
       <c r="C63" s="2"/>
       <c r="D63" t="s" s="2">
@@ -9135,7 +9227,7 @@
         <v>35</v>
       </c>
       <c r="G63" t="s" s="2">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="H63" t="s" s="2">
         <v>37</v>
@@ -9150,10 +9242,10 @@
         <v>173</v>
       </c>
       <c r="L63" t="s" s="2">
-        <v>416</v>
+        <v>386</v>
       </c>
       <c r="M63" t="s" s="2">
-        <v>417</v>
+        <v>387</v>
       </c>
       <c r="N63" t="s" s="2">
         <v>267</v>
@@ -9185,10 +9277,10 @@
         <v>282</v>
       </c>
       <c r="Y63" t="s" s="2">
-        <v>418</v>
+        <v>388</v>
       </c>
       <c r="Z63" t="s" s="2">
-        <v>419</v>
+        <v>37</v>
       </c>
       <c r="AA63" t="s" s="2">
         <v>37</v>
@@ -9206,13 +9298,13 @@
         <v>37</v>
       </c>
       <c r="AF63" t="s" s="2">
-        <v>415</v>
+        <v>385</v>
       </c>
       <c r="AG63" t="s" s="2">
         <v>35</v>
       </c>
       <c r="AH63" t="s" s="2">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="AI63" t="s" s="2">
         <v>59</v>
@@ -9221,7 +9313,7 @@
         <v>60</v>
       </c>
       <c r="AK63" t="s" s="2">
-        <v>420</v>
+        <v>389</v>
       </c>
       <c r="AL63" t="s" s="2">
         <v>271</v>
@@ -9230,18 +9322,18 @@
         <v>272</v>
       </c>
       <c r="AN63" t="s" s="2">
-        <v>421</v>
+        <v>390</v>
       </c>
       <c r="AO63" t="s" s="2">
-        <v>422</v>
+        <v>37</v>
       </c>
     </row>
     <row r="64" hidden="true">
       <c r="A64" t="s" s="2">
-        <v>423</v>
+        <v>391</v>
       </c>
       <c r="B64" t="s" s="2">
-        <v>423</v>
+        <v>391</v>
       </c>
       <c r="C64" s="2"/>
       <c r="D64" t="s" s="2">
@@ -9255,25 +9347,25 @@
         <v>36</v>
       </c>
       <c r="H64" t="s" s="2">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="I64" t="s" s="2">
         <v>37</v>
       </c>
       <c r="J64" t="s" s="2">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="K64" t="s" s="2">
-        <v>424</v>
+        <v>173</v>
       </c>
       <c r="L64" t="s" s="2">
-        <v>425</v>
+        <v>392</v>
       </c>
       <c r="M64" t="s" s="2">
-        <v>426</v>
+        <v>393</v>
       </c>
       <c r="N64" t="s" s="2">
-        <v>427</v>
+        <v>267</v>
       </c>
       <c r="O64" s="2"/>
       <c r="P64" t="s" s="2">
@@ -9299,13 +9391,13 @@
         <v>37</v>
       </c>
       <c r="X64" t="s" s="2">
-        <v>37</v>
+        <v>178</v>
       </c>
       <c r="Y64" t="s" s="2">
-        <v>37</v>
+        <v>394</v>
       </c>
       <c r="Z64" t="s" s="2">
-        <v>37</v>
+        <v>395</v>
       </c>
       <c r="AA64" t="s" s="2">
         <v>37</v>
@@ -9323,7 +9415,7 @@
         <v>37</v>
       </c>
       <c r="AF64" t="s" s="2">
-        <v>423</v>
+        <v>391</v>
       </c>
       <c r="AG64" t="s" s="2">
         <v>35</v>
@@ -9338,13 +9430,13 @@
         <v>60</v>
       </c>
       <c r="AK64" t="s" s="2">
-        <v>428</v>
+        <v>396</v>
       </c>
       <c r="AL64" t="s" s="2">
-        <v>61</v>
+        <v>271</v>
       </c>
       <c r="AM64" t="s" s="2">
-        <v>429</v>
+        <v>272</v>
       </c>
       <c r="AN64" t="s" s="2">
         <v>37</v>
@@ -9355,10 +9447,10 @@
     </row>
     <row r="65" hidden="true">
       <c r="A65" t="s" s="2">
-        <v>430</v>
+        <v>397</v>
       </c>
       <c r="B65" t="s" s="2">
-        <v>430</v>
+        <v>397</v>
       </c>
       <c r="C65" s="2"/>
       <c r="D65" t="s" s="2">
@@ -9369,10 +9461,10 @@
         <v>35</v>
       </c>
       <c r="G65" t="s" s="2">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="H65" t="s" s="2">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="I65" t="s" s="2">
         <v>37</v>
@@ -9381,15 +9473,17 @@
         <v>37</v>
       </c>
       <c r="K65" t="s" s="2">
-        <v>431</v>
+        <v>398</v>
       </c>
       <c r="L65" t="s" s="2">
-        <v>432</v>
+        <v>399</v>
       </c>
       <c r="M65" t="s" s="2">
-        <v>433</v>
-      </c>
-      <c r="N65" s="2"/>
+        <v>400</v>
+      </c>
+      <c r="N65" t="s" s="2">
+        <v>401</v>
+      </c>
       <c r="O65" s="2"/>
       <c r="P65" t="s" s="2">
         <v>37</v>
@@ -9438,13 +9532,13 @@
         <v>37</v>
       </c>
       <c r="AF65" t="s" s="2">
-        <v>430</v>
+        <v>397</v>
       </c>
       <c r="AG65" t="s" s="2">
         <v>35</v>
       </c>
       <c r="AH65" t="s" s="2">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="AI65" t="s" s="2">
         <v>59</v>
@@ -9453,7 +9547,7 @@
         <v>60</v>
       </c>
       <c r="AK65" t="s" s="2">
-        <v>434</v>
+        <v>402</v>
       </c>
       <c r="AL65" t="s" s="2">
         <v>37</v>
@@ -9462,7 +9556,7 @@
         <v>68</v>
       </c>
       <c r="AN65" t="s" s="2">
-        <v>435</v>
+        <v>403</v>
       </c>
       <c r="AO65" t="s" s="2">
         <v>37</v>
@@ -9470,41 +9564,43 @@
     </row>
     <row r="66" hidden="true">
       <c r="A66" t="s" s="2">
-        <v>436</v>
+        <v>404</v>
       </c>
       <c r="B66" t="s" s="2">
-        <v>436</v>
+        <v>404</v>
       </c>
       <c r="C66" s="2"/>
       <c r="D66" t="s" s="2">
-        <v>37</v>
+        <v>405</v>
       </c>
       <c r="E66" s="2"/>
       <c r="F66" t="s" s="2">
         <v>35</v>
       </c>
       <c r="G66" t="s" s="2">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="H66" t="s" s="2">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="I66" t="s" s="2">
         <v>37</v>
       </c>
       <c r="J66" t="s" s="2">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="K66" t="s" s="2">
-        <v>151</v>
+        <v>406</v>
       </c>
       <c r="L66" t="s" s="2">
-        <v>152</v>
+        <v>407</v>
       </c>
       <c r="M66" t="s" s="2">
-        <v>153</v>
-      </c>
-      <c r="N66" s="2"/>
+        <v>408</v>
+      </c>
+      <c r="N66" t="s" s="2">
+        <v>409</v>
+      </c>
       <c r="O66" s="2"/>
       <c r="P66" t="s" s="2">
         <v>37</v>
@@ -9553,53 +9649,53 @@
         <v>37</v>
       </c>
       <c r="AF66" t="s" s="2">
-        <v>154</v>
+        <v>404</v>
       </c>
       <c r="AG66" t="s" s="2">
         <v>35</v>
       </c>
       <c r="AH66" t="s" s="2">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="AI66" t="s" s="2">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="AJ66" t="s" s="2">
-        <v>37</v>
+        <v>219</v>
       </c>
       <c r="AK66" t="s" s="2">
-        <v>37</v>
+        <v>410</v>
       </c>
       <c r="AL66" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AM66" t="s" s="2">
-        <v>68</v>
+        <v>411</v>
       </c>
       <c r="AN66" t="s" s="2">
-        <v>37</v>
+        <v>412</v>
       </c>
       <c r="AO66" t="s" s="2">
-        <v>37</v>
+        <v>413</v>
       </c>
     </row>
     <row r="67" hidden="true">
       <c r="A67" t="s" s="2">
-        <v>437</v>
+        <v>414</v>
       </c>
       <c r="B67" t="s" s="2">
-        <v>437</v>
+        <v>414</v>
       </c>
       <c r="C67" s="2"/>
       <c r="D67" t="s" s="2">
-        <v>94</v>
+        <v>415</v>
       </c>
       <c r="E67" s="2"/>
       <c r="F67" t="s" s="2">
         <v>35</v>
       </c>
       <c r="G67" t="s" s="2">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="H67" t="s" s="2">
         <v>37</v>
@@ -9608,19 +9704,19 @@
         <v>37</v>
       </c>
       <c r="J67" t="s" s="2">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="K67" t="s" s="2">
-        <v>95</v>
+        <v>204</v>
       </c>
       <c r="L67" t="s" s="2">
-        <v>96</v>
+        <v>416</v>
       </c>
       <c r="M67" t="s" s="2">
-        <v>157</v>
+        <v>417</v>
       </c>
       <c r="N67" t="s" s="2">
-        <v>98</v>
+        <v>207</v>
       </c>
       <c r="O67" s="2"/>
       <c r="P67" t="s" s="2">
@@ -9658,90 +9754,88 @@
         <v>37</v>
       </c>
       <c r="AB67" t="s" s="2">
-        <v>99</v>
+        <v>37</v>
       </c>
       <c r="AC67" t="s" s="2">
-        <v>100</v>
+        <v>37</v>
       </c>
       <c r="AD67" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AE67" t="s" s="2">
-        <v>101</v>
+        <v>37</v>
       </c>
       <c r="AF67" t="s" s="2">
-        <v>158</v>
+        <v>414</v>
       </c>
       <c r="AG67" t="s" s="2">
         <v>35</v>
       </c>
       <c r="AH67" t="s" s="2">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="AI67" t="s" s="2">
         <v>59</v>
       </c>
       <c r="AJ67" t="s" s="2">
-        <v>103</v>
+        <v>209</v>
       </c>
       <c r="AK67" t="s" s="2">
-        <v>37</v>
+        <v>418</v>
       </c>
       <c r="AL67" t="s" s="2">
-        <v>37</v>
+        <v>419</v>
       </c>
       <c r="AM67" t="s" s="2">
-        <v>61</v>
+        <v>420</v>
       </c>
       <c r="AN67" t="s" s="2">
-        <v>37</v>
+        <v>421</v>
       </c>
       <c r="AO67" t="s" s="2">
-        <v>37</v>
+        <v>422</v>
       </c>
     </row>
     <row r="68" hidden="true">
       <c r="A68" t="s" s="2">
-        <v>438</v>
+        <v>423</v>
       </c>
       <c r="B68" t="s" s="2">
-        <v>438</v>
+        <v>423</v>
       </c>
       <c r="C68" s="2"/>
       <c r="D68" t="s" s="2">
-        <v>439</v>
+        <v>37</v>
       </c>
       <c r="E68" s="2"/>
       <c r="F68" t="s" s="2">
         <v>35</v>
       </c>
       <c r="G68" t="s" s="2">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="H68" t="s" s="2">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="I68" t="s" s="2">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="J68" t="s" s="2">
         <v>48</v>
       </c>
       <c r="K68" t="s" s="2">
-        <v>95</v>
+        <v>214</v>
       </c>
       <c r="L68" t="s" s="2">
-        <v>440</v>
+        <v>424</v>
       </c>
       <c r="M68" t="s" s="2">
-        <v>441</v>
+        <v>425</v>
       </c>
       <c r="N68" t="s" s="2">
-        <v>98</v>
-      </c>
-      <c r="O68" t="s" s="2">
-        <v>132</v>
-      </c>
+        <v>244</v>
+      </c>
+      <c r="O68" s="2"/>
       <c r="P68" t="s" s="2">
         <v>37</v>
       </c>
@@ -9789,42 +9883,42 @@
         <v>37</v>
       </c>
       <c r="AF68" t="s" s="2">
-        <v>442</v>
+        <v>423</v>
       </c>
       <c r="AG68" t="s" s="2">
         <v>35</v>
       </c>
       <c r="AH68" t="s" s="2">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="AI68" t="s" s="2">
         <v>59</v>
       </c>
       <c r="AJ68" t="s" s="2">
-        <v>103</v>
+        <v>219</v>
       </c>
       <c r="AK68" t="s" s="2">
-        <v>37</v>
+        <v>426</v>
       </c>
       <c r="AL68" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AM68" t="s" s="2">
-        <v>61</v>
+        <v>427</v>
       </c>
       <c r="AN68" t="s" s="2">
-        <v>37</v>
+        <v>428</v>
       </c>
       <c r="AO68" t="s" s="2">
-        <v>37</v>
+        <v>429</v>
       </c>
     </row>
     <row r="69" hidden="true">
       <c r="A69" t="s" s="2">
-        <v>443</v>
+        <v>430</v>
       </c>
       <c r="B69" t="s" s="2">
-        <v>443</v>
+        <v>430</v>
       </c>
       <c r="C69" s="2"/>
       <c r="D69" t="s" s="2">
@@ -9832,7 +9926,7 @@
       </c>
       <c r="E69" s="2"/>
       <c r="F69" t="s" s="2">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="G69" t="s" s="2">
         <v>47</v>
@@ -9844,19 +9938,19 @@
         <v>37</v>
       </c>
       <c r="J69" t="s" s="2">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="K69" t="s" s="2">
-        <v>151</v>
+        <v>431</v>
       </c>
       <c r="L69" t="s" s="2">
-        <v>444</v>
+        <v>432</v>
       </c>
       <c r="M69" t="s" s="2">
-        <v>445</v>
+        <v>433</v>
       </c>
       <c r="N69" t="s" s="2">
-        <v>237</v>
+        <v>244</v>
       </c>
       <c r="O69" s="2"/>
       <c r="P69" t="s" s="2">
@@ -9906,10 +10000,10 @@
         <v>37</v>
       </c>
       <c r="AF69" t="s" s="2">
-        <v>443</v>
+        <v>430</v>
       </c>
       <c r="AG69" t="s" s="2">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="AH69" t="s" s="2">
         <v>47</v>
@@ -9918,30 +10012,30 @@
         <v>59</v>
       </c>
       <c r="AJ69" t="s" s="2">
-        <v>60</v>
+        <v>219</v>
       </c>
       <c r="AK69" t="s" s="2">
-        <v>446</v>
+        <v>434</v>
       </c>
       <c r="AL69" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AM69" t="s" s="2">
-        <v>68</v>
+        <v>435</v>
       </c>
       <c r="AN69" t="s" s="2">
-        <v>447</v>
+        <v>436</v>
       </c>
       <c r="AO69" t="s" s="2">
-        <v>37</v>
+        <v>429</v>
       </c>
     </row>
     <row r="70" hidden="true">
       <c r="A70" t="s" s="2">
-        <v>448</v>
+        <v>437</v>
       </c>
       <c r="B70" t="s" s="2">
-        <v>448</v>
+        <v>437</v>
       </c>
       <c r="C70" s="2"/>
       <c r="D70" t="s" s="2">
@@ -9952,28 +10046,28 @@
         <v>35</v>
       </c>
       <c r="G70" t="s" s="2">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="H70" t="s" s="2">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="I70" t="s" s="2">
         <v>37</v>
       </c>
       <c r="J70" t="s" s="2">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="K70" t="s" s="2">
-        <v>173</v>
+        <v>438</v>
       </c>
       <c r="L70" t="s" s="2">
-        <v>449</v>
+        <v>439</v>
       </c>
       <c r="M70" t="s" s="2">
-        <v>450</v>
+        <v>440</v>
       </c>
       <c r="N70" t="s" s="2">
-        <v>267</v>
+        <v>244</v>
       </c>
       <c r="O70" s="2"/>
       <c r="P70" t="s" s="2">
@@ -10023,42 +10117,42 @@
         <v>37</v>
       </c>
       <c r="AF70" t="s" s="2">
-        <v>448</v>
+        <v>437</v>
       </c>
       <c r="AG70" t="s" s="2">
         <v>35</v>
       </c>
       <c r="AH70" t="s" s="2">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="AI70" t="s" s="2">
         <v>59</v>
       </c>
       <c r="AJ70" t="s" s="2">
-        <v>60</v>
+        <v>219</v>
       </c>
       <c r="AK70" t="s" s="2">
-        <v>451</v>
+        <v>441</v>
       </c>
       <c r="AL70" t="s" s="2">
-        <v>271</v>
+        <v>37</v>
       </c>
       <c r="AM70" t="s" s="2">
-        <v>272</v>
+        <v>435</v>
       </c>
       <c r="AN70" t="s" s="2">
-        <v>452</v>
+        <v>442</v>
       </c>
       <c r="AO70" t="s" s="2">
-        <v>37</v>
+        <v>443</v>
       </c>
     </row>
     <row r="71" hidden="true">
       <c r="A71" t="s" s="2">
-        <v>453</v>
+        <v>444</v>
       </c>
       <c r="B71" t="s" s="2">
-        <v>453</v>
+        <v>444</v>
       </c>
       <c r="C71" s="2"/>
       <c r="D71" t="s" s="2">
@@ -10078,19 +10172,19 @@
         <v>37</v>
       </c>
       <c r="J71" t="s" s="2">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="K71" t="s" s="2">
-        <v>151</v>
+        <v>173</v>
       </c>
       <c r="L71" t="s" s="2">
-        <v>454</v>
+        <v>445</v>
       </c>
       <c r="M71" t="s" s="2">
-        <v>455</v>
+        <v>446</v>
       </c>
       <c r="N71" t="s" s="2">
-        <v>237</v>
+        <v>267</v>
       </c>
       <c r="O71" s="2"/>
       <c r="P71" t="s" s="2">
@@ -10116,13 +10210,13 @@
         <v>37</v>
       </c>
       <c r="X71" t="s" s="2">
-        <v>37</v>
+        <v>282</v>
       </c>
       <c r="Y71" t="s" s="2">
-        <v>37</v>
+        <v>447</v>
       </c>
       <c r="Z71" t="s" s="2">
-        <v>37</v>
+        <v>448</v>
       </c>
       <c r="AA71" t="s" s="2">
         <v>37</v>
@@ -10140,7 +10234,7 @@
         <v>37</v>
       </c>
       <c r="AF71" t="s" s="2">
-        <v>453</v>
+        <v>444</v>
       </c>
       <c r="AG71" t="s" s="2">
         <v>35</v>
@@ -10155,27 +10249,27 @@
         <v>60</v>
       </c>
       <c r="AK71" t="s" s="2">
-        <v>456</v>
+        <v>449</v>
       </c>
       <c r="AL71" t="s" s="2">
-        <v>37</v>
+        <v>271</v>
       </c>
       <c r="AM71" t="s" s="2">
-        <v>68</v>
+        <v>272</v>
       </c>
       <c r="AN71" t="s" s="2">
-        <v>457</v>
+        <v>450</v>
       </c>
       <c r="AO71" t="s" s="2">
-        <v>37</v>
+        <v>451</v>
       </c>
     </row>
     <row r="72" hidden="true">
       <c r="A72" t="s" s="2">
-        <v>458</v>
+        <v>452</v>
       </c>
       <c r="B72" t="s" s="2">
-        <v>458</v>
+        <v>452</v>
       </c>
       <c r="C72" s="2"/>
       <c r="D72" t="s" s="2">
@@ -10198,15 +10292,17 @@
         <v>37</v>
       </c>
       <c r="K72" t="s" s="2">
-        <v>431</v>
+        <v>453</v>
       </c>
       <c r="L72" t="s" s="2">
-        <v>459</v>
+        <v>454</v>
       </c>
       <c r="M72" t="s" s="2">
-        <v>460</v>
-      </c>
-      <c r="N72" s="2"/>
+        <v>455</v>
+      </c>
+      <c r="N72" t="s" s="2">
+        <v>456</v>
+      </c>
       <c r="O72" s="2"/>
       <c r="P72" t="s" s="2">
         <v>37</v>
@@ -10255,7 +10351,7 @@
         <v>37</v>
       </c>
       <c r="AF72" t="s" s="2">
-        <v>458</v>
+        <v>452</v>
       </c>
       <c r="AG72" t="s" s="2">
         <v>35</v>
@@ -10270,13 +10366,13 @@
         <v>60</v>
       </c>
       <c r="AK72" t="s" s="2">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="AL72" t="s" s="2">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="AM72" t="s" s="2">
-        <v>68</v>
+        <v>458</v>
       </c>
       <c r="AN72" t="s" s="2">
         <v>37</v>
@@ -10287,10 +10383,10 @@
     </row>
     <row r="73" hidden="true">
       <c r="A73" t="s" s="2">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="B73" t="s" s="2">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="C73" s="2"/>
       <c r="D73" t="s" s="2">
@@ -10301,7 +10397,7 @@
         <v>35</v>
       </c>
       <c r="G73" t="s" s="2">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="H73" t="s" s="2">
         <v>37</v>
@@ -10313,13 +10409,13 @@
         <v>37</v>
       </c>
       <c r="K73" t="s" s="2">
-        <v>151</v>
+        <v>460</v>
       </c>
       <c r="L73" t="s" s="2">
-        <v>152</v>
+        <v>461</v>
       </c>
       <c r="M73" t="s" s="2">
-        <v>153</v>
+        <v>462</v>
       </c>
       <c r="N73" s="2"/>
       <c r="O73" s="2"/>
@@ -10370,22 +10466,22 @@
         <v>37</v>
       </c>
       <c r="AF73" t="s" s="2">
-        <v>154</v>
+        <v>459</v>
       </c>
       <c r="AG73" t="s" s="2">
         <v>35</v>
       </c>
       <c r="AH73" t="s" s="2">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="AI73" t="s" s="2">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="AJ73" t="s" s="2">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="AK73" t="s" s="2">
-        <v>37</v>
+        <v>463</v>
       </c>
       <c r="AL73" t="s" s="2">
         <v>37</v>
@@ -10394,7 +10490,7 @@
         <v>68</v>
       </c>
       <c r="AN73" t="s" s="2">
-        <v>37</v>
+        <v>464</v>
       </c>
       <c r="AO73" t="s" s="2">
         <v>37</v>
@@ -10402,21 +10498,21 @@
     </row>
     <row r="74" hidden="true">
       <c r="A74" t="s" s="2">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="B74" t="s" s="2">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="C74" s="2"/>
       <c r="D74" t="s" s="2">
-        <v>94</v>
+        <v>37</v>
       </c>
       <c r="E74" s="2"/>
       <c r="F74" t="s" s="2">
         <v>35</v>
       </c>
       <c r="G74" t="s" s="2">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="H74" t="s" s="2">
         <v>37</v>
@@ -10428,17 +10524,15 @@
         <v>37</v>
       </c>
       <c r="K74" t="s" s="2">
-        <v>95</v>
+        <v>151</v>
       </c>
       <c r="L74" t="s" s="2">
-        <v>96</v>
+        <v>152</v>
       </c>
       <c r="M74" t="s" s="2">
-        <v>157</v>
-      </c>
-      <c r="N74" t="s" s="2">
-        <v>98</v>
-      </c>
+        <v>153</v>
+      </c>
+      <c r="N74" s="2"/>
       <c r="O74" s="2"/>
       <c r="P74" t="s" s="2">
         <v>37</v>
@@ -10475,31 +10569,31 @@
         <v>37</v>
       </c>
       <c r="AB74" t="s" s="2">
-        <v>99</v>
+        <v>37</v>
       </c>
       <c r="AC74" t="s" s="2">
-        <v>100</v>
+        <v>37</v>
       </c>
       <c r="AD74" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AE74" t="s" s="2">
-        <v>101</v>
+        <v>37</v>
       </c>
       <c r="AF74" t="s" s="2">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="AG74" t="s" s="2">
         <v>35</v>
       </c>
       <c r="AH74" t="s" s="2">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="AI74" t="s" s="2">
-        <v>59</v>
+        <v>37</v>
       </c>
       <c r="AJ74" t="s" s="2">
-        <v>103</v>
+        <v>37</v>
       </c>
       <c r="AK74" t="s" s="2">
         <v>37</v>
@@ -10508,7 +10602,7 @@
         <v>37</v>
       </c>
       <c r="AM74" t="s" s="2">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="AN74" t="s" s="2">
         <v>37</v>
@@ -10519,14 +10613,14 @@
     </row>
     <row r="75" hidden="true">
       <c r="A75" t="s" s="2">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="B75" t="s" s="2">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="C75" s="2"/>
       <c r="D75" t="s" s="2">
-        <v>439</v>
+        <v>94</v>
       </c>
       <c r="E75" s="2"/>
       <c r="F75" t="s" s="2">
@@ -10539,26 +10633,24 @@
         <v>37</v>
       </c>
       <c r="I75" t="s" s="2">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="J75" t="s" s="2">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="K75" t="s" s="2">
         <v>95</v>
       </c>
       <c r="L75" t="s" s="2">
-        <v>440</v>
+        <v>96</v>
       </c>
       <c r="M75" t="s" s="2">
-        <v>441</v>
+        <v>157</v>
       </c>
       <c r="N75" t="s" s="2">
         <v>98</v>
       </c>
-      <c r="O75" t="s" s="2">
-        <v>132</v>
-      </c>
+      <c r="O75" s="2"/>
       <c r="P75" t="s" s="2">
         <v>37</v>
       </c>
@@ -10594,19 +10686,19 @@
         <v>37</v>
       </c>
       <c r="AB75" t="s" s="2">
-        <v>37</v>
+        <v>99</v>
       </c>
       <c r="AC75" t="s" s="2">
-        <v>37</v>
+        <v>100</v>
       </c>
       <c r="AD75" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AE75" t="s" s="2">
-        <v>37</v>
+        <v>101</v>
       </c>
       <c r="AF75" t="s" s="2">
-        <v>442</v>
+        <v>158</v>
       </c>
       <c r="AG75" t="s" s="2">
         <v>35</v>
@@ -10638,44 +10730,46 @@
     </row>
     <row r="76" hidden="true">
       <c r="A76" t="s" s="2">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="B76" t="s" s="2">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="C76" s="2"/>
       <c r="D76" t="s" s="2">
-        <v>37</v>
+        <v>468</v>
       </c>
       <c r="E76" s="2"/>
       <c r="F76" t="s" s="2">
         <v>35</v>
       </c>
       <c r="G76" t="s" s="2">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="H76" t="s" s="2">
         <v>37</v>
       </c>
       <c r="I76" t="s" s="2">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="J76" t="s" s="2">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="K76" t="s" s="2">
-        <v>151</v>
+        <v>95</v>
       </c>
       <c r="L76" t="s" s="2">
-        <v>466</v>
+        <v>469</v>
       </c>
       <c r="M76" t="s" s="2">
-        <v>467</v>
+        <v>470</v>
       </c>
       <c r="N76" t="s" s="2">
-        <v>237</v>
-      </c>
-      <c r="O76" s="2"/>
+        <v>98</v>
+      </c>
+      <c r="O76" t="s" s="2">
+        <v>132</v>
+      </c>
       <c r="P76" t="s" s="2">
         <v>37</v>
       </c>
@@ -10723,28 +10817,28 @@
         <v>37</v>
       </c>
       <c r="AF76" t="s" s="2">
-        <v>465</v>
+        <v>471</v>
       </c>
       <c r="AG76" t="s" s="2">
         <v>35</v>
       </c>
       <c r="AH76" t="s" s="2">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="AI76" t="s" s="2">
         <v>59</v>
       </c>
       <c r="AJ76" t="s" s="2">
-        <v>60</v>
+        <v>103</v>
       </c>
       <c r="AK76" t="s" s="2">
-        <v>468</v>
+        <v>37</v>
       </c>
       <c r="AL76" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AM76" t="s" s="2">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="AN76" t="s" s="2">
         <v>37</v>
@@ -10755,10 +10849,10 @@
     </row>
     <row r="77" hidden="true">
       <c r="A77" t="s" s="2">
-        <v>469</v>
+        <v>472</v>
       </c>
       <c r="B77" t="s" s="2">
-        <v>469</v>
+        <v>472</v>
       </c>
       <c r="C77" s="2"/>
       <c r="D77" t="s" s="2">
@@ -10766,7 +10860,7 @@
       </c>
       <c r="E77" s="2"/>
       <c r="F77" t="s" s="2">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="G77" t="s" s="2">
         <v>47</v>
@@ -10781,16 +10875,16 @@
         <v>37</v>
       </c>
       <c r="K77" t="s" s="2">
-        <v>173</v>
+        <v>151</v>
       </c>
       <c r="L77" t="s" s="2">
-        <v>470</v>
+        <v>473</v>
       </c>
       <c r="M77" t="s" s="2">
-        <v>471</v>
+        <v>474</v>
       </c>
       <c r="N77" t="s" s="2">
-        <v>267</v>
+        <v>237</v>
       </c>
       <c r="O77" s="2"/>
       <c r="P77" t="s" s="2">
@@ -10816,34 +10910,34 @@
         <v>37</v>
       </c>
       <c r="X77" t="s" s="2">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="Y77" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="Z77" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AA77" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AB77" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AC77" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AD77" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AE77" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AF77" t="s" s="2">
         <v>472</v>
       </c>
-      <c r="Z77" t="s" s="2">
-        <v>473</v>
-      </c>
-      <c r="AA77" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AB77" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AC77" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AD77" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AE77" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AF77" t="s" s="2">
-        <v>469</v>
-      </c>
       <c r="AG77" t="s" s="2">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="AH77" t="s" s="2">
         <v>47</v>
@@ -10855,23 +10949,957 @@
         <v>60</v>
       </c>
       <c r="AK77" t="s" s="2">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="AL77" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AM77" t="s" s="2">
+        <v>68</v>
+      </c>
+      <c r="AN77" t="s" s="2">
+        <v>476</v>
+      </c>
+      <c r="AO77" t="s" s="2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="78" hidden="true">
+      <c r="A78" t="s" s="2">
+        <v>477</v>
+      </c>
+      <c r="B78" t="s" s="2">
+        <v>477</v>
+      </c>
+      <c r="C78" s="2"/>
+      <c r="D78" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="E78" s="2"/>
+      <c r="F78" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="G78" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="H78" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="I78" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="J78" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="K78" t="s" s="2">
+        <v>173</v>
+      </c>
+      <c r="L78" t="s" s="2">
+        <v>478</v>
+      </c>
+      <c r="M78" t="s" s="2">
+        <v>479</v>
+      </c>
+      <c r="N78" t="s" s="2">
+        <v>267</v>
+      </c>
+      <c r="O78" s="2"/>
+      <c r="P78" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="Q78" s="2"/>
+      <c r="R78" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="S78" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="T78" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="U78" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="V78" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="W78" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="X78" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="Y78" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="Z78" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AA78" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AB78" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AC78" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AD78" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AE78" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AF78" t="s" s="2">
+        <v>477</v>
+      </c>
+      <c r="AG78" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AH78" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="AI78" t="s" s="2">
+        <v>59</v>
+      </c>
+      <c r="AJ78" t="s" s="2">
+        <v>60</v>
+      </c>
+      <c r="AK78" t="s" s="2">
+        <v>480</v>
+      </c>
+      <c r="AL78" t="s" s="2">
         <v>271</v>
       </c>
-      <c r="AM77" t="s" s="2">
+      <c r="AM78" t="s" s="2">
         <v>272</v>
       </c>
-      <c r="AN77" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AO77" t="s" s="2">
+      <c r="AN78" t="s" s="2">
+        <v>481</v>
+      </c>
+      <c r="AO78" t="s" s="2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="79" hidden="true">
+      <c r="A79" t="s" s="2">
+        <v>482</v>
+      </c>
+      <c r="B79" t="s" s="2">
+        <v>482</v>
+      </c>
+      <c r="C79" s="2"/>
+      <c r="D79" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="E79" s="2"/>
+      <c r="F79" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="G79" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="H79" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="I79" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="J79" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="K79" t="s" s="2">
+        <v>151</v>
+      </c>
+      <c r="L79" t="s" s="2">
+        <v>483</v>
+      </c>
+      <c r="M79" t="s" s="2">
+        <v>484</v>
+      </c>
+      <c r="N79" t="s" s="2">
+        <v>237</v>
+      </c>
+      <c r="O79" s="2"/>
+      <c r="P79" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="Q79" s="2"/>
+      <c r="R79" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="S79" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="T79" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="U79" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="V79" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="W79" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="X79" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="Y79" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="Z79" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AA79" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AB79" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AC79" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AD79" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AE79" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AF79" t="s" s="2">
+        <v>482</v>
+      </c>
+      <c r="AG79" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AH79" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="AI79" t="s" s="2">
+        <v>59</v>
+      </c>
+      <c r="AJ79" t="s" s="2">
+        <v>60</v>
+      </c>
+      <c r="AK79" t="s" s="2">
+        <v>485</v>
+      </c>
+      <c r="AL79" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AM79" t="s" s="2">
+        <v>68</v>
+      </c>
+      <c r="AN79" t="s" s="2">
+        <v>486</v>
+      </c>
+      <c r="AO79" t="s" s="2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="80" hidden="true">
+      <c r="A80" t="s" s="2">
+        <v>487</v>
+      </c>
+      <c r="B80" t="s" s="2">
+        <v>487</v>
+      </c>
+      <c r="C80" s="2"/>
+      <c r="D80" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="E80" s="2"/>
+      <c r="F80" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="G80" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="H80" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="I80" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="J80" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="K80" t="s" s="2">
+        <v>460</v>
+      </c>
+      <c r="L80" t="s" s="2">
+        <v>488</v>
+      </c>
+      <c r="M80" t="s" s="2">
+        <v>489</v>
+      </c>
+      <c r="N80" s="2"/>
+      <c r="O80" s="2"/>
+      <c r="P80" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="Q80" s="2"/>
+      <c r="R80" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="S80" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="T80" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="U80" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="V80" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="W80" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="X80" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="Y80" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="Z80" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AA80" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AB80" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AC80" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AD80" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AE80" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AF80" t="s" s="2">
+        <v>487</v>
+      </c>
+      <c r="AG80" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AH80" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="AI80" t="s" s="2">
+        <v>59</v>
+      </c>
+      <c r="AJ80" t="s" s="2">
+        <v>60</v>
+      </c>
+      <c r="AK80" t="s" s="2">
+        <v>490</v>
+      </c>
+      <c r="AL80" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AM80" t="s" s="2">
+        <v>68</v>
+      </c>
+      <c r="AN80" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AO80" t="s" s="2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="81" hidden="true">
+      <c r="A81" t="s" s="2">
+        <v>491</v>
+      </c>
+      <c r="B81" t="s" s="2">
+        <v>491</v>
+      </c>
+      <c r="C81" s="2"/>
+      <c r="D81" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="E81" s="2"/>
+      <c r="F81" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="G81" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="H81" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="I81" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="J81" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="K81" t="s" s="2">
+        <v>151</v>
+      </c>
+      <c r="L81" t="s" s="2">
+        <v>152</v>
+      </c>
+      <c r="M81" t="s" s="2">
+        <v>153</v>
+      </c>
+      <c r="N81" s="2"/>
+      <c r="O81" s="2"/>
+      <c r="P81" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="Q81" s="2"/>
+      <c r="R81" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="S81" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="T81" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="U81" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="V81" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="W81" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="X81" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="Y81" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="Z81" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AA81" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AB81" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AC81" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AD81" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AE81" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AF81" t="s" s="2">
+        <v>154</v>
+      </c>
+      <c r="AG81" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AH81" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="AI81" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AJ81" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AK81" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AL81" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AM81" t="s" s="2">
+        <v>68</v>
+      </c>
+      <c r="AN81" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AO81" t="s" s="2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="82" hidden="true">
+      <c r="A82" t="s" s="2">
+        <v>492</v>
+      </c>
+      <c r="B82" t="s" s="2">
+        <v>492</v>
+      </c>
+      <c r="C82" s="2"/>
+      <c r="D82" t="s" s="2">
+        <v>94</v>
+      </c>
+      <c r="E82" s="2"/>
+      <c r="F82" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="G82" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="H82" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="I82" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="J82" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="K82" t="s" s="2">
+        <v>95</v>
+      </c>
+      <c r="L82" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="M82" t="s" s="2">
+        <v>157</v>
+      </c>
+      <c r="N82" t="s" s="2">
+        <v>98</v>
+      </c>
+      <c r="O82" s="2"/>
+      <c r="P82" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="Q82" s="2"/>
+      <c r="R82" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="S82" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="T82" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="U82" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="V82" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="W82" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="X82" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="Y82" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="Z82" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AA82" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AB82" t="s" s="2">
+        <v>99</v>
+      </c>
+      <c r="AC82" t="s" s="2">
+        <v>100</v>
+      </c>
+      <c r="AD82" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AE82" t="s" s="2">
+        <v>101</v>
+      </c>
+      <c r="AF82" t="s" s="2">
+        <v>158</v>
+      </c>
+      <c r="AG82" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AH82" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="AI82" t="s" s="2">
+        <v>59</v>
+      </c>
+      <c r="AJ82" t="s" s="2">
+        <v>103</v>
+      </c>
+      <c r="AK82" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AL82" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AM82" t="s" s="2">
+        <v>61</v>
+      </c>
+      <c r="AN82" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AO82" t="s" s="2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="83" hidden="true">
+      <c r="A83" t="s" s="2">
+        <v>493</v>
+      </c>
+      <c r="B83" t="s" s="2">
+        <v>493</v>
+      </c>
+      <c r="C83" s="2"/>
+      <c r="D83" t="s" s="2">
+        <v>468</v>
+      </c>
+      <c r="E83" s="2"/>
+      <c r="F83" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="G83" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="H83" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="I83" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="J83" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="K83" t="s" s="2">
+        <v>95</v>
+      </c>
+      <c r="L83" t="s" s="2">
+        <v>469</v>
+      </c>
+      <c r="M83" t="s" s="2">
+        <v>470</v>
+      </c>
+      <c r="N83" t="s" s="2">
+        <v>98</v>
+      </c>
+      <c r="O83" t="s" s="2">
+        <v>132</v>
+      </c>
+      <c r="P83" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="Q83" s="2"/>
+      <c r="R83" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="S83" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="T83" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="U83" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="V83" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="W83" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="X83" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="Y83" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="Z83" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AA83" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AB83" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AC83" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AD83" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AE83" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AF83" t="s" s="2">
+        <v>471</v>
+      </c>
+      <c r="AG83" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AH83" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="AI83" t="s" s="2">
+        <v>59</v>
+      </c>
+      <c r="AJ83" t="s" s="2">
+        <v>103</v>
+      </c>
+      <c r="AK83" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AL83" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AM83" t="s" s="2">
+        <v>61</v>
+      </c>
+      <c r="AN83" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AO83" t="s" s="2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="84" hidden="true">
+      <c r="A84" t="s" s="2">
+        <v>494</v>
+      </c>
+      <c r="B84" t="s" s="2">
+        <v>494</v>
+      </c>
+      <c r="C84" s="2"/>
+      <c r="D84" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="E84" s="2"/>
+      <c r="F84" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="G84" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="H84" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="I84" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="J84" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="K84" t="s" s="2">
+        <v>151</v>
+      </c>
+      <c r="L84" t="s" s="2">
+        <v>495</v>
+      </c>
+      <c r="M84" t="s" s="2">
+        <v>496</v>
+      </c>
+      <c r="N84" t="s" s="2">
+        <v>237</v>
+      </c>
+      <c r="O84" s="2"/>
+      <c r="P84" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="Q84" s="2"/>
+      <c r="R84" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="S84" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="T84" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="U84" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="V84" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="W84" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="X84" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="Y84" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="Z84" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AA84" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AB84" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AC84" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AD84" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AE84" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AF84" t="s" s="2">
+        <v>494</v>
+      </c>
+      <c r="AG84" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AH84" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="AI84" t="s" s="2">
+        <v>59</v>
+      </c>
+      <c r="AJ84" t="s" s="2">
+        <v>60</v>
+      </c>
+      <c r="AK84" t="s" s="2">
+        <v>497</v>
+      </c>
+      <c r="AL84" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AM84" t="s" s="2">
+        <v>68</v>
+      </c>
+      <c r="AN84" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AO84" t="s" s="2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="85" hidden="true">
+      <c r="A85" t="s" s="2">
+        <v>498</v>
+      </c>
+      <c r="B85" t="s" s="2">
+        <v>498</v>
+      </c>
+      <c r="C85" s="2"/>
+      <c r="D85" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="E85" s="2"/>
+      <c r="F85" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="G85" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="H85" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="I85" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="J85" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="K85" t="s" s="2">
+        <v>173</v>
+      </c>
+      <c r="L85" t="s" s="2">
+        <v>499</v>
+      </c>
+      <c r="M85" t="s" s="2">
+        <v>500</v>
+      </c>
+      <c r="N85" t="s" s="2">
+        <v>267</v>
+      </c>
+      <c r="O85" s="2"/>
+      <c r="P85" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="Q85" s="2"/>
+      <c r="R85" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="S85" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="T85" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="U85" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="V85" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="W85" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="X85" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Y85" t="s" s="2">
+        <v>501</v>
+      </c>
+      <c r="Z85" t="s" s="2">
+        <v>502</v>
+      </c>
+      <c r="AA85" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AB85" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AC85" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AD85" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AE85" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AF85" t="s" s="2">
+        <v>498</v>
+      </c>
+      <c r="AG85" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AH85" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="AI85" t="s" s="2">
+        <v>59</v>
+      </c>
+      <c r="AJ85" t="s" s="2">
+        <v>60</v>
+      </c>
+      <c r="AK85" t="s" s="2">
+        <v>503</v>
+      </c>
+      <c r="AL85" t="s" s="2">
+        <v>271</v>
+      </c>
+      <c r="AM85" t="s" s="2">
+        <v>272</v>
+      </c>
+      <c r="AN85" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AO85" t="s" s="2">
         <v>37</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AO77">
+  <autoFilter ref="A1:AO85">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -10881,7 +11909,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI76">
+  <conditionalFormatting sqref="A2:AI84">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>